<commit_message>
sample assets xls changed
</commit_message>
<xml_diff>
--- a/uploads/sampleFile/Sample_asset_data.xlsx
+++ b/uploads/sampleFile/Sample_asset_data.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="24960" yWindow="2505" windowWidth="24240" windowHeight="11355" tabRatio="178"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="24240" windowHeight="7995" tabRatio="178"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="83">
   <si>
     <t>Visual</t>
   </si>
@@ -48,46 +48,15 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">subAsets </t>
-  </si>
-  <si>
     <t>UOM</t>
   </si>
   <si>
-    <t>Inspection Type</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Observation</t>
-  </si>
-  <si>
     <t>Repair</t>
   </si>
   <si>
     <t>GEO Facing</t>
   </si>
   <si>
-    <t>freq in
- month</t>
-  </si>
-  <si>
-    <t>freq 
-(in hours)</t>
-  </si>
-  <si>
-    <t>lifespan
-(in month)</t>
-  </si>
-  <si>
-    <t>lifespan
-(in hours)</t>
-  </si>
-  <si>
-    <t>infonet_status</t>
-  </si>
-  <si>
     <t>nos</t>
   </si>
   <si>
@@ -115,75 +84,42 @@
     <t>CORNER ROOF POST FOR STANDING SEAM</t>
   </si>
   <si>
-    <t>No Corrosion/ Rust/ Pitting Should Be FoundNo Sharp Edges/deformation/corrosion/crack Should Be FoundFasteners Are Tightened</t>
-  </si>
-  <si>
-    <t>Light Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingDeformation FoundOkCrack FoundDamage FoundDistortion FoundPitting FoundRust Found</t>
-  </si>
-  <si>
     <t>FA6021200</t>
   </si>
   <si>
     <t>ROOF TOP ANCHOR POST</t>
   </si>
   <si>
-    <t>No Sharp Edges/deformation/corrosion/crack Should Be FoundNo Corrosion/ Rust/ Pitting Should Be FoundFasteners Are Tightened</t>
-  </si>
-  <si>
-    <t>Light Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingDeformation FoundOkSharp Edges FoundCrack FoundDamage FoundDistortion FoundPitting FoundRust Found</t>
-  </si>
-  <si>
     <t>FA2020300</t>
   </si>
   <si>
     <t>UBOLT</t>
   </si>
   <si>
-    <t>No Corrosion/ Rust/ Pitting Should Be FoundNo Sharp Edges/deformation/corrosion/crack Should Be Found</t>
-  </si>
-  <si>
-    <t>Entire Component MissingLight Corrosion FoundHeavy Corrosion FoundDeformation FoundOkSharp Edges FoundCrack FoundDamage FoundDistortion FoundPitting FoundRust Found</t>
-  </si>
-  <si>
     <t>FA6022300</t>
   </si>
   <si>
     <t>INTERMEDIATE POST FOR STANDING SEAM</t>
   </si>
   <si>
-    <t>Fasteners LooseLight Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingOkSharp Edges FoundCrack FoundDamage FoundDistortion FoundPitting FoundRust FoundComponent Deformed</t>
-  </si>
-  <si>
     <t>FA6022200</t>
   </si>
   <si>
     <t>EXTRIMITY POST FOR STANDING SEAM ROOF</t>
   </si>
   <si>
-    <t>Fasteners LooseLight Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingDeformation FoundOkSharp Edges FoundCrack FoundPitting FoundRust Found</t>
-  </si>
-  <si>
     <t>FA6022000</t>
   </si>
   <si>
     <t>INTERMEDIATE POST FOR METALLIC ROOF</t>
   </si>
   <si>
-    <t>Fasteners LooseLight Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingDeformation FoundOkSharp Edges FoundCrack FoundDamage FoundDistortion FoundPitting FoundRust FoundComponent Deformed</t>
-  </si>
-  <si>
     <t>FA6021900</t>
   </si>
   <si>
     <t>EXTREMITY POST FOR METALLIC SHEET</t>
   </si>
   <si>
-    <t>No Corrosion/ Rust/ Pitting Should Be FoundNo Sharp Edges/deformation/corrosion/crack Should Be FoundNo Damage Or Parts Are Missing And  Fasteneres Are Not Loose</t>
-  </si>
-  <si>
-    <t>Fasteners LooseLight Corrosion FoundHeavy Corrosion FoundNut Or Bolts MissingDeformation FoundOkSharp Edges FoundCrack FoundDamage FoundPitting FoundRust FoundDeterioration Found</t>
-  </si>
-  <si>
     <t>DT-SL</t>
   </si>
   <si>
@@ -205,9 +141,6 @@
     <t>mtr</t>
   </si>
   <si>
-    <t>No Cut/nicks/tear Should Be  FoundNo Fraying/ Discoloration Should Be Found</t>
-  </si>
-  <si>
     <t>Orientation Of Mounting Bracket Incorrect Or BentDamaged Or Torn</t>
   </si>
   <si>
@@ -217,9 +150,6 @@
     <t>Test data to check</t>
   </si>
   <si>
-    <t>No Cut/nicks/tear Should Be  FoundNo Uneven Thickness/  Undue Stretching Should Be Found</t>
-  </si>
-  <si>
     <t>Damaged Or TornFasteners Loose</t>
   </si>
   <si>
@@ -238,25 +168,115 @@
     <t>VERTEX PULLEY TYPE CABLE GUIDE PN7000(04)</t>
   </si>
   <si>
-    <t>No Corrosion/ Rust/ Pitting Should Be FoundNo Distoration/ Broken/ Damage/ Sharp Edges/ Crack Should Be FoundThe Strength Should Be 10kn</t>
-  </si>
-  <si>
-    <t>Distortion FoundDistortion FoundCrack FoundPitting FoundLight Corrosion FoundHeavy Corrosion FoundEntire Component MissingRust FoundSharp Edges FoundBrokenSharp Edges Found</t>
-  </si>
-  <si>
     <t>CABLE EXTREMITY-SS316 (8MMDIA)</t>
   </si>
   <si>
-    <t>No Corrosion/ Rust/ Pitting Should Be FoundShould Not Be Damaged/deshapedNo Sharp Edges Should Be FoundNo Crack Should Be Observed</t>
-  </si>
-  <si>
-    <t>Damage FoundRust FoundLight Corrosion FoundHeavy Corrosion FoundPitting Found</t>
-  </si>
-  <si>
     <t>TEST, TESTING12</t>
   </si>
   <si>
     <t>TEST, TESTING16,TESTING167,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Assets </t>
+  </si>
+  <si>
+    <t>Type of Inspection</t>
+  </si>
+  <si>
+    <t>Frequency of Product (in hours)</t>
+  </si>
+  <si>
+    <t>Frequency of Product(in month)</t>
+  </si>
+  <si>
+    <t>Life span of Product (in month)</t>
+  </si>
+  <si>
+    <t>Standards</t>
+  </si>
+  <si>
+    <t>EC Type Certificate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>EN358:2000</t>
+  </si>
+  <si>
+    <t>EN795:2012,TS16415:2013</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>SATRA N°0321 Wyndham Way, Telford Way, Kettering, Northamptonshire, NN6 8SD, UK</t>
+  </si>
+  <si>
+    <t>Notified Body ( certification )</t>
+  </si>
+  <si>
+    <t>Notified Body  
+( Article 11B)</t>
+  </si>
+  <si>
+    <t>SGS United Kingdom Ltd., N° 0120 Unit 202B, Worle Parkway, Weston-super-Mare, BS22 6WA, United Kingdom</t>
+  </si>
+  <si>
+    <t>technical generation test 12 modify</t>
+  </si>
+  <si>
+    <t>Frequency of Periodic
+ Maintenance (in Days)</t>
+  </si>
+  <si>
+    <t>KnowledgeTree
+_status</t>
+  </si>
+  <si>
+    <t>Life span of 
+ Product (in hours)</t>
+  </si>
+  <si>
+    <t>EN361:2002</t>
+  </si>
+  <si>
+    <t>No Corrosion/ Rust/ Pitting Should Be Found##No Sharp Edges/deformation/corrosion/crack Should Be Found##Fasteners Are Tightened</t>
+  </si>
+  <si>
+    <t>No Cut/nicks/tear Should Be  Found##No Fraying/ Discoloration Should Be Found</t>
+  </si>
+  <si>
+    <t>No Cut/nicks/tear Should Be  Found##No Uneven Thickness/  Undue Stretching Should Be Found</t>
+  </si>
+  <si>
+    <t>No Corrosion/ Rust/ Pitting Should Be Found##No Distoration/ Broken/ Damage/ Sharp Edges/ Crack Should Be Found##The Strength Should Be 10kn</t>
+  </si>
+  <si>
+    <t>No Corrosion/ Rust/ Pitting Should Be Found##Should Not Be Damaged/deshaped##No Sharp Edges Should Be Found##No Crack Should Be Observed</t>
+  </si>
+  <si>
+    <t>No Corrosion/ Rust/ Pitting Should Be Found##No Sharp Edges/deformation/corrosion/crack Should Be Found##No Damage Or Parts Are Missing And  Fasteneres Are Not Loose</t>
+  </si>
+  <si>
+    <t>No Sharp Edges/deformation/corrosion/crack Should Be Found##No Corrosion/ Rust/ Pitting Should Be Found##Fasteners Are Tightened</t>
+  </si>
+  <si>
+    <t>Light Corrosion Found##Heavy Corrosion Found##Nut Or Bolts Missing##Deformation Found Ok##Crack Found##Damage Found##Distortion Found##Pitting Found##Rust Found</t>
+  </si>
+  <si>
+    <t>Damage Found##Rust Found##Light Corrosion Found##Heavy Corrosion Found##Pitting Found</t>
+  </si>
+  <si>
+    <t>Expected Result
+(Result is seperated BY ## )</t>
+  </si>
+  <si>
+    <t>Observation
+(Observation is seperated BY ## )</t>
   </si>
 </sst>
 </file>
@@ -704,16 +724,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,7 +782,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,6 +790,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1112,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1125,17 +1148,24 @@
     <col min="3" max="3" width="49.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="8" width="34" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="156.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="195.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="75">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="60">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1146,76 +1176,94 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
+      <c r="L1" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:22">
       <c r="A2" s="4">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L2" s="4">
         <v>12</v>
@@ -1230,42 +1278,58 @@
         <v>3423</v>
       </c>
       <c r="P2" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="4">
         <v>1</v>
       </c>
+      <c r="R2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:22">
       <c r="A3" s="4">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L3" s="4">
         <v>12</v>
@@ -1280,40 +1344,58 @@
         <v>3423</v>
       </c>
       <c r="P3" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="4">
         <v>1</v>
       </c>
+      <c r="R3" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:22">
       <c r="A4" s="4">
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L4" s="4">
         <v>12</v>
@@ -1328,42 +1410,60 @@
         <v>3423</v>
       </c>
       <c r="P4" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="4">
         <v>1</v>
       </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:22">
       <c r="A5" s="4">
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4">
         <v>12</v>
@@ -1378,40 +1478,58 @@
         <v>3423</v>
       </c>
       <c r="P5" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="4">
         <v>1</v>
       </c>
+      <c r="R5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:22">
       <c r="A6" s="4">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L6" s="4">
         <v>12</v>
@@ -1426,40 +1544,58 @@
         <v>3423</v>
       </c>
       <c r="P6" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="4">
         <v>1</v>
       </c>
+      <c r="R6" t="s">
+        <v>71</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:22">
       <c r="A7" s="4">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L7" s="4">
         <v>12</v>
@@ -1474,40 +1610,58 @@
         <v>3423</v>
       </c>
       <c r="P7" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q7" s="4">
         <v>1</v>
       </c>
+      <c r="R7" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:22">
       <c r="A8" s="4">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L8" s="4">
         <v>12</v>
@@ -1522,42 +1676,60 @@
         <v>3423</v>
       </c>
       <c r="P8" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q8" s="4">
         <v>1</v>
       </c>
+      <c r="R8" t="s">
+        <v>61</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" t="s">
+        <v>67</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:22">
       <c r="A9" s="4">
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L9" s="4">
         <v>12</v>
@@ -1572,40 +1744,58 @@
         <v>3423</v>
       </c>
       <c r="P9" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q9" s="4">
         <v>1</v>
       </c>
+      <c r="R9" t="s">
+        <v>61</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:22">
       <c r="A10" s="4">
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L10" s="4">
         <v>12</v>
@@ -1620,42 +1810,60 @@
         <v>3423</v>
       </c>
       <c r="P10" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q10" s="4">
         <v>1</v>
       </c>
+      <c r="R10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:22">
       <c r="A11" s="4">
         <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L11" s="4">
         <v>12</v>
@@ -1670,40 +1878,56 @@
         <v>3423</v>
       </c>
       <c r="P11" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q11" s="4">
         <v>1</v>
       </c>
+      <c r="R11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:22">
       <c r="A12" s="4">
         <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L12" s="4">
         <v>12</v>
@@ -1718,40 +1942,54 @@
         <v>3423</v>
       </c>
       <c r="P12" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q12" s="4">
         <v>1</v>
       </c>
+      <c r="R12" t="s">
+        <v>61</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:22">
       <c r="A13" s="4">
         <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L13" s="4">
         <v>12</v>
@@ -1766,10 +2004,24 @@
         <v>3423</v>
       </c>
       <c r="P13" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q13" s="4">
         <v>1</v>
       </c>
+      <c r="R13" t="s">
+        <v>61</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:22">
       <c r="A14" s="4">
         <v>22</v>
       </c>
@@ -1777,31 +2029,31 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L14" s="4">
         <v>12</v>
@@ -1816,10 +2068,24 @@
         <v>3423</v>
       </c>
       <c r="P14" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q14" s="4">
         <v>1</v>
       </c>
+      <c r="R14" t="s">
+        <v>61</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:22">
       <c r="A15" s="4">
         <v>23</v>
       </c>
@@ -1827,29 +2093,29 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L15" s="4">
         <v>12</v>
@@ -1863,8 +2129,20 @@
       <c r="O15" s="4">
         <v>3423</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4">
         <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>